<commit_message>
Task Manager project with all test cases and xml file
</commit_message>
<xml_diff>
--- a/TaskManager_Technical_Analysis_Report.xlsx
+++ b/TaskManager_Technical_Analysis_Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="900" windowWidth="20730" windowHeight="11760" activeTab="2"/>
+    <workbookView xWindow="1140" yWindow="900" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TaskManager_Entities" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="130">
   <si>
     <t xml:space="preserve">Problem Statement </t>
   </si>
@@ -320,60 +320,9 @@
     <t>MongoBookDBContext_GetCollection_ValidName_Success()</t>
   </si>
   <si>
-    <t xml:space="preserve">BusinessTestFor_NewTaskGroup() : Task </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BusinessTestFor_NewTask() : Task </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BusinessTestFor_EditTask() : Task </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BusinessTestFor_GetAllTask() : Task </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BusinessTestFor_GetTaskDashboard() : Task </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ExceptionTestFor_GetAllTask_Fail()  : Task </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ExceptionTestFor_GetTaskDashboard_Fail()  : Task </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ExceptionTestFor_EditTask_Fail()  : Task </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ExceptionTestFor_NewTaskGroup_Fail()  : Task </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ExceptionTestFor_NewTask_Fail()  : Task </t>
-  </si>
-  <si>
-    <t>BoundaryTestFor_TaskNameRequiredAsync()</t>
-  </si>
-  <si>
-    <t>BoundaryTestFor_TaskStartDateRequiredAsync()</t>
-  </si>
-  <si>
-    <t>BoundaryTestFor_TaskEndDateRequiredAsync()</t>
-  </si>
-  <si>
-    <t>BoundaryTestFor_TaskEndDateGreaterThanTaskStartDateAsync()</t>
-  </si>
-  <si>
-    <t>BoundaryTestFor_TaskColorCodeRequireAsync()</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> GetAllTask() : ActionResult&lt;IEnumerable&lt;TaskItem&gt;&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve"> NewTask(TaskItem newtask) : Task&lt;ActionResult&lt;String&gt;&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve"> EditTask(TaskItem task) : Task&lt;ActionResult&lt;String&gt;&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">  GetAllTaskGroups() : Task&lt;ActionResult&lt;IEnumerable&lt;TaskGroup&gt;&gt;&gt;</t>
   </si>
   <si>
@@ -386,9 +335,6 @@
     <t xml:space="preserve">GetAllTaskGroup() : List&lt;TaskGroup&gt; </t>
   </si>
   <si>
-    <t>EditTask( TaskItem task) : String</t>
-  </si>
-  <si>
     <t>NewTaskGroup( TaskGroup taskGroup) : String</t>
   </si>
   <si>
@@ -396,6 +342,84 @@
   </si>
   <si>
     <t>GetAllTask() : List&lt;TaskItem&gt;</t>
+  </si>
+  <si>
+    <t>TestCases</t>
+  </si>
+  <si>
+    <t>EditTask( TaskItem task) : long</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EditTask(TaskItem task) : Task&lt;ActionResult&lt;long&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GetAllTask() : ActionResult&lt;List&lt;TaskItem&gt;&gt;</t>
+  </si>
+  <si>
+    <t>FunctionalTestFor_GetAllTaskGroups_Api</t>
+  </si>
+  <si>
+    <t>BusinessTestFor_NewTask_Successed</t>
+  </si>
+  <si>
+    <t>BusinessTestFor_NewTaskGroup_Successed</t>
+  </si>
+  <si>
+    <t>BusinessTestFor_EditTask_Successed</t>
+  </si>
+  <si>
+    <t>BusinessTestFor_GetAllTask_Successed</t>
+  </si>
+  <si>
+    <t>BusinessTestFor_GetTaskDashboard_Successed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BusinessTestFor_GetAllTaskGroups_Successed</t>
+  </si>
+  <si>
+    <t>ExceptionTestFor_NewTask_FailWithNullException</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ExceptionTestFor_NewTaskGroup_FailWithException </t>
+  </si>
+  <si>
+    <t>ExceptionTestFor_EditTask_FailWithException</t>
+  </si>
+  <si>
+    <t>ExceptionTestFor_GetAllTask_FailWithException</t>
+  </si>
+  <si>
+    <t>ExceptionTestFor_GetTaskDashboard_FailWithException</t>
+  </si>
+  <si>
+    <t>ExceptionTestFor_GetAllTaskGroups_FailWithException</t>
+  </si>
+  <si>
+    <t>BoundaryTestFor_TaskStartDateRequiredAsync</t>
+  </si>
+  <si>
+    <t>BoundaryTestFor_TaskName_Required</t>
+  </si>
+  <si>
+    <t>BoundaryTestFor_TaskEndDate_Required</t>
+  </si>
+  <si>
+    <t>BoundaryTestFor_TaskEndDateGreaterThanTaskStartDate</t>
+  </si>
+  <si>
+    <t>BoundaryTestFor_TaskColorCode_Require</t>
+  </si>
+  <si>
+    <t>BoundaryTestFor_TaskGroup_Require</t>
+  </si>
+  <si>
+    <t>BoundaryTestFor_GroupName_Require</t>
+  </si>
+  <si>
+    <t>BoundaryTestFor_GroupIsActive_Require</t>
+  </si>
+  <si>
+    <t>BoundaryTestFor_GroupColor_Require</t>
   </si>
 </sst>
 </file>
@@ -498,10 +522,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -808,7 +832,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -819,8 +843,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:W37"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A19" zoomScale="85" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -831,6 +855,9 @@
     <col min="4" max="4" width="41.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="57.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="41.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="35.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="26.25" x14ac:dyDescent="0.4">
@@ -875,30 +902,30 @@
       <c r="A5" s="5"/>
     </row>
     <row r="6" spans="1:23" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
-      <c r="V6" s="8"/>
-      <c r="W6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -1035,7 +1062,9 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="6"/>
+      <c r="B16" s="7" t="s">
+        <v>104</v>
+      </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
     </row>
@@ -1074,30 +1103,30 @@
     </row>
     <row r="28" spans="1:23" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A28" s="3"/>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
-      <c r="T28" s="8"/>
-      <c r="U28" s="8"/>
-      <c r="V28" s="8"/>
-      <c r="W28" s="8"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9"/>
     </row>
     <row r="29" spans="1:23" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A29" s="4" t="s">
@@ -1185,42 +1214,54 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>65</v>
       </c>
@@ -1239,8 +1280,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:W37"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1294,30 +1335,30 @@
       <c r="A5" s="5"/>
     </row>
     <row r="6" spans="1:23" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
-      <c r="V6" s="8"/>
-      <c r="W6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -1477,30 +1518,30 @@
     </row>
     <row r="28" spans="1:23" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A28" s="3"/>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
-      <c r="T28" s="8"/>
-      <c r="U28" s="8"/>
-      <c r="V28" s="8"/>
-      <c r="W28" s="8"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9"/>
     </row>
     <row r="29" spans="1:23" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A29" s="4" t="s">
@@ -1633,19 +1674,18 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:W37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="A16" zoomScale="85" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="57.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="70.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="46.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="51.875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="34.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31.625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1692,30 +1732,30 @@
       <c r="A5" s="5"/>
     </row>
     <row r="6" spans="1:23" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
-      <c r="V6" s="8"/>
-      <c r="W6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -1804,46 +1844,46 @@
       <c r="A11" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>115</v>
+      <c r="B11" s="8" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>119</v>
+      <c r="B12" s="8" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>118</v>
+      <c r="B13" s="8" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>121</v>
+      <c r="B14" s="8" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>116</v>
+      <c r="B15" s="8" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="9" t="s">
-        <v>117</v>
+      <c r="B16" s="8" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
@@ -1881,30 +1921,30 @@
     </row>
     <row r="28" spans="1:23" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A28" s="3"/>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
-      <c r="T28" s="8"/>
-      <c r="U28" s="8"/>
-      <c r="V28" s="8"/>
-      <c r="W28" s="8"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9"/>
     </row>
     <row r="29" spans="1:23" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A29" s="4" t="s">
@@ -1992,57 +2032,63 @@
         <v>21</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>65</v>
       </c>
@@ -2062,8 +2108,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:W37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A19" zoomScale="85" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2073,7 +2119,7 @@
     <col min="3" max="3" width="35.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="40.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="26.25" x14ac:dyDescent="0.4">
@@ -2118,34 +2164,34 @@
       <c r="A5" s="5"/>
     </row>
     <row r="6" spans="1:23" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
-      <c r="V6" s="8"/>
-      <c r="W6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="G7" t="s">
         <v>9</v>
@@ -2218,15 +2264,15 @@
       <c r="A11" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>112</v>
+      <c r="B11" s="8" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2234,30 +2280,30 @@
       <c r="A13" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>113</v>
+      <c r="B13" s="8" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>111</v>
+      <c r="B14" s="8" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="9" t="s">
-        <v>114</v>
+      <c r="B16" s="8" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
@@ -2295,30 +2341,30 @@
     </row>
     <row r="28" spans="1:23" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A28" s="3"/>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
-      <c r="T28" s="8"/>
-      <c r="U28" s="8"/>
-      <c r="V28" s="8"/>
-      <c r="W28" s="8"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9"/>
     </row>
     <row r="29" spans="1:23" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A29" s="4" t="s">
@@ -2406,7 +2452,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>22</v>
       </c>
@@ -2425,23 +2471,26 @@
       <c r="F33" s="7" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>65</v>
       </c>

</xml_diff>